<commit_message>
bg value l and hue difference graphs
</commit_message>
<xml_diff>
--- a/Data/Difference In L Value.xlsx
+++ b/Data/Difference In L Value.xlsx
@@ -11,12 +11,16 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$47:$AI$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$AP$2:$BA$2</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>Lumist</t>
   </si>
@@ -27,7 +31,28 @@
     <t>Ideal</t>
   </si>
   <si>
-    <t>Measured</t>
+    <t xml:space="preserve">Captured </t>
+  </si>
+  <si>
+    <t>Catured</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>lumist</t>
+  </si>
+  <si>
+    <t>acc</t>
+  </si>
+  <si>
+    <t>measured</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
@@ -587,9 +612,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.8268934711739378E-2"/>
+          <c:y val="2.9936005795188823E-2"/>
+          <c:w val="0.71763868671766673"/>
+          <c:h val="0.90251658452428118"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -598,11 +633,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$1</c:f>
+              <c:f>Sheet1!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ideal</c:v>
+                  <c:v>Captured </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -610,167 +645,332 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>0.274175951657257</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3708797582862899</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7417595165725701</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.7357684291265203</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.4641215787700208</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.157550364361301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.760231648870301</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17.285082881441699</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19.7420591932039</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.139043572028001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24.482416760248601</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>26.7774381673444</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>29.028509630148999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>31.239363532919398</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>33.413200390998497</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>35.552791671337303</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>37.660558090522102</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>39.738630230206802</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>41.7888961531891</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43.813039297706297</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45.812568988870296</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>47.788845265682497</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>49.743099276495997</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>51.676450180349299</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>53.589919264710403</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>55.4844418246023</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>57.360877225658697</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>59.220017482019998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>61.062594610629297</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>62.889286970436302</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>64.700724754063202</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>66.497494767573102</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>68.280144608909097</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>70.049186335723306</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>71.805099697480699</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>73.548334994008698</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>75.279315612383996</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>76.998440285692496</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>78.706085110360704</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>80.402605353137304</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>82.088337074152903</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>83.763598588631893</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>85.428691786604205</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>87.083903327267606</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>88.729505722377297</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>90.365758321121405</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>91.992908207308204</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>96.822045162958503</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>95.220831693995095</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>98.415036972298196</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>93.611191018306599</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$55</c:f>
+              <c:f>Sheet1!$B$2:$B$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>0.274175951657257</c:v>
+                  <c:v>10.776862781141901</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3708797582862899</c:v>
+                  <c:v>2.3485800000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.7417595165725701</c:v>
+                  <c:v>4.6971600000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.7357684291265203</c:v>
+                  <c:v>2.1679200000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.4641215787700208</c:v>
+                  <c:v>4.6971600000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.157550364361301</c:v>
+                  <c:v>5.60046</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14.760231648870301</c:v>
+                  <c:v>8.5677767886783798</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17.285082881441699</c:v>
+                  <c:v>10.6309369261204</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>19.7420591932039</c:v>
+                  <c:v>14.624142025665201</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22.139043572028001</c:v>
+                  <c:v>15.901597716120101</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>24.482416760248601</c:v>
+                  <c:v>19.6388751779558</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>26.7774381673444</c:v>
+                  <c:v>19.5155562847184</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>29.028509630148999</c:v>
+                  <c:v>21.5426180714291</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>31.239363532919398</c:v>
+                  <c:v>24.064254063450299</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>33.413200390998497</c:v>
+                  <c:v>27.7367242396869</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>35.552791671337303</c:v>
+                  <c:v>28.511695617097899</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>37.660558090522102</c:v>
+                  <c:v>30.7358958701886</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>39.738630230206802</c:v>
+                  <c:v>33.752738504003197</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>41.7888961531891</c:v>
+                  <c:v>35.887849022101797</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>43.813039297706297</c:v>
+                  <c:v>37.626193479594797</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>45.812568988870296</c:v>
+                  <c:v>39.563622668770698</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>47.788845265682497</c:v>
+                  <c:v>42.657583051835601</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>49.743099276495997</c:v>
+                  <c:v>43.241502429265601</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>51.676450180349299</c:v>
+                  <c:v>45.852566230966303</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>53.589919264710403</c:v>
+                  <c:v>47.752030057102203</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>55.4844418246023</c:v>
+                  <c:v>49.965759282189097</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>57.360877225658697</c:v>
+                  <c:v>51.667192739674199</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>59.220017482019998</c:v>
+                  <c:v>53.416926278080098</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>61.062594610629297</c:v>
+                  <c:v>55.634399790935497</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>62.889286970436302</c:v>
+                  <c:v>57.530520047616399</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>64.700724754063202</c:v>
+                  <c:v>59.094463774282403</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>66.497494767573102</c:v>
+                  <c:v>61.089286206221303</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>68.280144608909097</c:v>
+                  <c:v>63.1440287463505</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>70.049186335723306</c:v>
+                  <c:v>64.9546334587952</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>71.805099697480699</c:v>
+                  <c:v>66.854756502700297</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>73.548334994008698</c:v>
+                  <c:v>68.4605212685819</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>75.279315612383996</c:v>
+                  <c:v>70.677442615378496</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>76.998440285692496</c:v>
+                  <c:v>72.355310294280699</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>78.706085110360704</c:v>
+                  <c:v>74.253688193184502</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>80.402605353137304</c:v>
+                  <c:v>75.940183170738095</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>82.088337074152903</c:v>
+                  <c:v>77.780438453810206</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>83.763598588631893</c:v>
+                  <c:v>79.471324230318899</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>85.428691786604205</c:v>
+                  <c:v>81.137443985067407</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>87.083903327267606</c:v>
+                  <c:v>82.961258398373403</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>88.729505722377297</c:v>
+                  <c:v>85.088148800481093</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>90.365758321121405</c:v>
+                  <c:v>86.657327858777904</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>91.992908207308204</c:v>
+                  <c:v>88.357019344668998</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>93.611191018306599</c:v>
+                  <c:v>93.878806202783693</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>95.220831693995095</c:v>
+                  <c:v>92.118339967250293</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>96.822045162958503</c:v>
+                  <c:v>95.526065888121096</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>98.415036972298196</c:v>
+                  <c:v>90.211035887826696</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>100</c:v>
+                  <c:v>97.381608124741504</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -782,11 +982,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Sheet1!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Measured</c:v>
+                  <c:v>Lumist</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -794,167 +994,332 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>0.274175951657257</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3708797582862899</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7417595165725701</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.7357684291265203</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.4641215787700208</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.157550364361301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.760231648870301</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17.285082881441699</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19.7420591932039</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.139043572028001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24.482416760248601</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>26.7774381673444</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>29.028509630148999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>31.239363532919398</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>33.413200390998497</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>35.552791671337303</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>37.660558090522102</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>39.738630230206802</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>41.7888961531891</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43.813039297706297</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45.812568988870296</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>47.788845265682497</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>49.743099276495997</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>51.676450180349299</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>53.589919264710403</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>55.4844418246023</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>57.360877225658697</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>59.220017482019998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>61.062594610629297</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>62.889286970436302</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>64.700724754063202</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>66.497494767573102</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>68.280144608909097</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>70.049186335723306</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>71.805099697480699</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>73.548334994008698</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>75.279315612383996</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>76.998440285692496</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>78.706085110360704</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>80.402605353137304</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>82.088337074152903</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>83.763598588631893</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>85.428691786604205</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>87.083903327267606</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>88.729505722377297</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>90.365758321121405</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>91.992908207308204</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>96.822045162958503</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>95.220831693995095</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>98.415036972298196</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>93.611191018306599</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$55</c:f>
+              <c:f>Sheet1!$C$2:$C$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>10.776862781141901</c:v>
+                  <c:v>0.18065999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3485800000000001</c:v>
+                  <c:v>1.1742900000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.6971600000000002</c:v>
+                  <c:v>3.79386</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.1679200000000001</c:v>
+                  <c:v>3.8841899999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.6971600000000002</c:v>
+                  <c:v>1.5356099999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.60046</c:v>
+                  <c:v>4.9681499999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.5677767886783798</c:v>
+                  <c:v>6.41343</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.6309369261204</c:v>
+                  <c:v>9.7197546792129295</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14.624142025665201</c:v>
+                  <c:v>7.9490400000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15.901597716120101</c:v>
+                  <c:v>12.351471710606701</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19.6388751779558</c:v>
+                  <c:v>15.007668446298201</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>19.5155562847184</c:v>
+                  <c:v>15.275914197399899</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>21.5426180714291</c:v>
+                  <c:v>18.5838453549134</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>24.064254063450299</c:v>
+                  <c:v>20.6736117900255</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>27.7367242396869</c:v>
+                  <c:v>21.0185249333875</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>28.511695617097899</c:v>
+                  <c:v>23.704473986455699</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>30.7358958701886</c:v>
+                  <c:v>26.9332707927881</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>33.752738504003197</c:v>
+                  <c:v>28.590338352372399</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>35.887849022101797</c:v>
+                  <c:v>28.772767250297498</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>37.626193479594797</c:v>
+                  <c:v>32.033485893305098</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>39.563622668770698</c:v>
+                  <c:v>33.541650948504497</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>42.657583051835601</c:v>
+                  <c:v>35.732785418318102</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>43.241502429265601</c:v>
+                  <c:v>37.316839705335802</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>45.852566230966303</c:v>
+                  <c:v>38.393150089069799</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>47.752030057102203</c:v>
+                  <c:v>39.981787274646699</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>49.965759282189097</c:v>
+                  <c:v>41.922563325806898</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>51.667192739674199</c:v>
+                  <c:v>43.988138099520903</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>53.416926278080098</c:v>
+                  <c:v>45.524429733063002</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>55.634399790935497</c:v>
+                  <c:v>47.287799776223999</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>57.530520047616399</c:v>
+                  <c:v>48.846860886126798</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>59.094463774282403</c:v>
+                  <c:v>50.144626099371898</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>61.089286206221303</c:v>
+                  <c:v>51.848515844615903</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>63.1440287463505</c:v>
+                  <c:v>53.824828511193402</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>64.9546334587952</c:v>
+                  <c:v>55.328918894917798</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>66.854756502700297</c:v>
+                  <c:v>57.250382665242199</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>68.4605212685819</c:v>
+                  <c:v>58.630275477922702</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>70.677442615378496</c:v>
+                  <c:v>60.346721989780299</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>72.355310294280699</c:v>
+                  <c:v>62.006380893723502</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>74.253688193184502</c:v>
+                  <c:v>63.786700463451702</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>75.940183170738095</c:v>
+                  <c:v>65.152625426819199</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>77.780438453810206</c:v>
+                  <c:v>66.778896034994403</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>79.471324230318899</c:v>
+                  <c:v>68.292432913162301</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>81.137443985067407</c:v>
+                  <c:v>70.140877448106806</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>82.961258398373403</c:v>
+                  <c:v>71.275806200509095</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>85.088148800481093</c:v>
+                  <c:v>73.200298416424104</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>86.657327858777904</c:v>
+                  <c:v>74.685956430130105</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>88.357019344668998</c:v>
+                  <c:v>75.995546602325504</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>90.211035887826696</c:v>
+                  <c:v>81.071228937973899</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>92.118339967250293</c:v>
+                  <c:v>79.379903910616605</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>93.878806202783693</c:v>
+                  <c:v>82.636111340414203</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>95.526065888121096</c:v>
+                  <c:v>78.122318625670104</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>97.381608124741504</c:v>
+                  <c:v>84.085377113407205</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -966,190 +1331,6 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Lumist</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$2:$C$55</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="54"/>
-                <c:pt idx="0">
-                  <c:v>0.18065999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.1742900000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.79386</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.8841899999999998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.5356099999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.9681499999999996</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6.41343</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9.7197546792129295</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7.9490400000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>12.351471710606701</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>15.007668446298201</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>15.275914197399899</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>18.5838453549134</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>20.6736117900255</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>21.0185249333875</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>23.704473986455699</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>26.9332707927881</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>28.590338352372399</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>28.772767250297498</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>32.033485893305098</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>33.541650948504497</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>35.732785418318102</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>37.316839705335802</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>38.393150089069799</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>39.981787274646699</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>41.922563325806898</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>43.988138099520903</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>45.524429733063002</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>47.287799776223999</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>48.846860886126798</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>50.144626099371898</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>51.848515844615903</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>53.824828511193402</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>55.328918894917798</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>57.250382665242199</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>58.630275477922702</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>60.346721989780299</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>62.006380893723502</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>63.786700463451702</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>65.152625426819199</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>66.778896034994403</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>68.292432913162301</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>70.140877448106806</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>71.275806200509095</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>73.200298416424104</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>74.685956430130105</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>75.995546602325504</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>78.122318625670104</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>79.379903910616605</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>81.071228937973899</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>82.636111340414203</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>84.085377113407205</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
               <c:f>Sheet1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -1159,15 +1340,189 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>0.274175951657257</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3708797582862899</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7417595165725701</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.7357684291265203</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.4641215787700208</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.157550364361301</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.760231648870301</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17.285082881441699</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19.7420591932039</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.139043572028001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24.482416760248601</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>26.7774381673444</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>29.028509630148999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>31.239363532919398</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>33.413200390998497</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>35.552791671337303</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>37.660558090522102</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>39.738630230206802</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>41.7888961531891</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>43.813039297706297</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45.812568988870296</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>47.788845265682497</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>49.743099276495997</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>51.676450180349299</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>53.589919264710403</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>55.4844418246023</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>57.360877225658697</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>59.220017482019998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>61.062594610629297</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>62.889286970436302</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>64.700724754063202</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>66.497494767573102</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>68.280144608909097</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>70.049186335723306</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>71.805099697480699</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>73.548334994008698</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>75.279315612383996</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>76.998440285692496</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>78.706085110360704</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>80.402605353137304</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>82.088337074152903</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>83.763598588631893</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>85.428691786604205</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>87.083903327267606</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>88.729505722377297</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>90.365758321121405</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>91.992908207308204</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>96.822045162958503</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>95.220831693995095</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>98.415036972298196</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>93.611191018306599</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$55</c:f>
+              <c:f>Sheet1!$D$2:$D$53</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="52"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1310,16 +1665,16 @@
                   <c:v>59.260174787056002</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>60.816914677161797</c:v>
+                  <c:v>63.565411097727697</c:v>
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>62.049110076728098</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>63.565411097727697</c:v>
+                  <c:v>64.403088913774198</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>64.403088913774198</c:v>
+                  <c:v>60.816914677161797</c:v>
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>65.694129808594397</c:v>
@@ -1339,41 +1694,715 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="65590784"/>
-        <c:axId val="65592320"/>
+        <c:axId val="61691776"/>
+        <c:axId val="654097792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="65590784"/>
+        <c:axId val="61691776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65592320"/>
+        <c:crossAx val="654097792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:tickLblSkip val="5"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65592320"/>
+        <c:axId val="654097792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Measure</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> L</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="61691776"/>
+        <c:crossesAt val="1"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.8268934711739378E-2"/>
+          <c:y val="2.9936005795188823E-2"/>
+          <c:w val="0.71763868671766673"/>
+          <c:h val="0.90251658452428118"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Y$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Catured</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$AP$3:$AP$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>24.151217137615198</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.911270827222801</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33.962258063326502</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38.9108388997441</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40.858774363473898</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42.513016739339498</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43.810561975230698</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>46.403220698567999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>52.826633416237897</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>52.930781940618502</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>53.705458975919498</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>54.322688581342597</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>58.330714001573597</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>58.594288513308797</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>62.803105697604003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>68.3412110813655</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>68.635025805353095</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>73.091809568476606</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>73.460038120237598</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>73.973784381781797</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>82.424217104485194</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>82.7944957735874</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>95.816325481331205</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Y$7:$Y$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>17.913580040012501</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31.339461447313099</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.354934388910799</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35.509328934257098</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37.792530135046803</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41.744535704265203</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41.834550714674997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43.150765072798499</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>51.7579755991502</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>52.310025166339798</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>51.557170758806201</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>52.7445915281059</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>56.319553627202303</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>57.065676205042799</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>61.771962973055899</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>67.121690575514293</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>67.798100176184406</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>72.206954570721905</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>72.670393280597295</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>72.613740508446696</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>82.852522013889995</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>82.710924759429204</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>97.4521674453065</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Z$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lumist</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$AP$3:$AP$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>24.151217137615198</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.911270827222801</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33.962258063326502</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38.9108388997441</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40.858774363473898</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42.513016739339498</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43.810561975230698</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>46.403220698567999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>52.826633416237897</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>52.930781940618502</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>53.705458975919498</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>54.322688581342597</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>58.330714001573597</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>58.594288513308797</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>62.803105697604003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>68.3412110813655</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>68.635025805353095</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>73.091809568476606</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>73.460038120237598</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>73.973784381781797</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>82.424217104485194</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>82.7944957735874</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>95.816325481331205</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Z$7:$Z$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>14.306480065276901</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.017431907081399</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25.693460563374899</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.942275621855298</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.364452848225802</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35.496252180982701</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34.916404346768402</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36.442330071055302</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44.2122094237901</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44.505769610168002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43.653732903271099</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43.973676156313601</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>47.456222555428603</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>48.780804319481902</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>53.236499913979998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>57.781999474018399</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>57.790494199513198</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>62.229008458145699</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>62.790814232688398</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>62.520762952460402</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>71.363000178237201</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>71.728079207486402</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>84.665480396724107</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$AA$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Phone</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$AP$3:$AP$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>24.151217137615198</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.911270827222801</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33.962258063326502</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38.9108388997441</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40.858774363473898</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42.513016739339498</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43.810561975230698</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>46.403220698567999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>52.826633416237897</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>52.930781940618502</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>53.705458975919498</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>54.322688581342597</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>58.330714001573597</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>58.594288513308797</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>62.803105697604003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>68.3412110813655</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>68.635025805353095</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>73.091809568476606</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>73.460038120237598</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>73.973784381781797</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>82.424217104485194</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>82.7944957735874</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>95.816325481331205</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AA$7:$AA$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>8.6726870460000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.264089650000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16.93031878</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.675250680000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22.525664219999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.412627430000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24.06425406</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25.283719820000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>31.316233050000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30.613827910000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>31.608791230000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30.725306570000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>32.943240250000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>34.482334369999997</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>37.487123910000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41.748003009999998</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>41.18961891</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>44.802764119999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>45.417334719999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>44.977400539999998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>51.5533705</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>51.578697480000002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>61.769095489999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="b"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="667112576"/>
+        <c:axId val="667114496"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="667112576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="in"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="667114496"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="5"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="667114496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Measure</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-CA" baseline="0"/>
+                  <a:t> L</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-CA"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65590784"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossAx val="667112576"/>
+        <c:crossesAt val="1"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1398,19 +2427,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:colOff>114299</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:rowOff>176211</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1420,6 +2449,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>68037</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>458562</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>42864</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1715,13 +2776,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:BA53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AH43" sqref="AH43"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1735,7 +2798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0.274175951657257</v>
       </c>
@@ -1748,8 +2811,50 @@
       <c r="D2" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>9</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1.3708797582862899</v>
       </c>
@@ -1762,8 +2867,50 @@
       <c r="D3" s="4">
         <v>3.9745200000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3" s="4">
+        <v>5</v>
+      </c>
+      <c r="AP3" s="4">
+        <v>24.151217137615198</v>
+      </c>
+      <c r="AQ3" s="4">
+        <v>0.68378038042568601</v>
+      </c>
+      <c r="AR3" s="4">
+        <v>-0.48486915906436101</v>
+      </c>
+      <c r="AS3" s="4">
+        <v>14.306480065276901</v>
+      </c>
+      <c r="AT3" s="4">
+        <v>8.4256558159653494</v>
+      </c>
+      <c r="AU3" s="4">
+        <v>-2.1294508723131198</v>
+      </c>
+      <c r="AV3" s="4">
+        <v>17.913580040012501</v>
+      </c>
+      <c r="AW3" s="4">
+        <v>0.28554726574042699</v>
+      </c>
+      <c r="AX3" s="4">
+        <v>-4.0945719467350301</v>
+      </c>
+      <c r="AY3" s="4">
+        <v>8.6726870460000001</v>
+      </c>
+      <c r="AZ3" s="4">
+        <v>-2.7879048069999999</v>
+      </c>
+      <c r="BA3" s="4">
+        <v>2.0793560379999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2.7417595165725701</v>
       </c>
@@ -1776,8 +2923,50 @@
       <c r="D4" s="4">
         <v>0.18065999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4" s="4">
+        <v>10</v>
+      </c>
+      <c r="AP4" s="4">
+        <v>32.911270827222801</v>
+      </c>
+      <c r="AQ4" s="4">
+        <v>24.7139871060205</v>
+      </c>
+      <c r="AR4" s="4">
+        <v>-51.448245354658901</v>
+      </c>
+      <c r="AS4" s="4">
+        <v>25.017431907081399</v>
+      </c>
+      <c r="AT4" s="4">
+        <v>22.193352039870199</v>
+      </c>
+      <c r="AU4" s="4">
+        <v>-48.553479341188101</v>
+      </c>
+      <c r="AV4" s="4">
+        <v>31.339461447313099</v>
+      </c>
+      <c r="AW4" s="4">
+        <v>32.583372471131497</v>
+      </c>
+      <c r="AX4" s="4">
+        <v>-58.937199536029802</v>
+      </c>
+      <c r="AY4" s="4">
+        <v>15.264089650000001</v>
+      </c>
+      <c r="AZ4" s="4">
+        <v>16.433664180000001</v>
+      </c>
+      <c r="BA4" s="4">
+        <v>-36.622390230000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>6.7357684291265203</v>
       </c>
@@ -1790,8 +2979,50 @@
       <c r="D5" s="4">
         <v>5.1488100000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G5" s="4">
+        <v>15</v>
+      </c>
+      <c r="H5" s="4">
+        <v>15</v>
+      </c>
+      <c r="AP5" s="4">
+        <v>33.962258063326502</v>
+      </c>
+      <c r="AQ5" s="4">
+        <v>23.4195165871866</v>
+      </c>
+      <c r="AR5" s="4">
+        <v>-22.210871318606301</v>
+      </c>
+      <c r="AS5" s="4">
+        <v>25.693460563374899</v>
+      </c>
+      <c r="AT5" s="4">
+        <v>23.2115841084956</v>
+      </c>
+      <c r="AU5" s="4">
+        <v>-22.4589424835805</v>
+      </c>
+      <c r="AV5" s="4">
+        <v>31.354934388910799</v>
+      </c>
+      <c r="AW5" s="4">
+        <v>28.355198138318499</v>
+      </c>
+      <c r="AX5" s="4">
+        <v>-28.1859364938956</v>
+      </c>
+      <c r="AY5" s="4">
+        <v>16.93031878</v>
+      </c>
+      <c r="AZ5" s="4">
+        <v>18.913645540000001</v>
+      </c>
+      <c r="BA5" s="4">
+        <v>-11.54879049</v>
+      </c>
+    </row>
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>9.4641215787700208</v>
       </c>
@@ -1804,8 +3035,59 @@
       <c r="D6" s="4">
         <v>3.5228700000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G6" s="4">
+        <v>20</v>
+      </c>
+      <c r="H6" s="4">
+        <v>20</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP6" s="4">
+        <v>38.9108388997441</v>
+      </c>
+      <c r="AQ6" s="4">
+        <v>5.8028281869348898E-3</v>
+      </c>
+      <c r="AR6" s="4">
+        <v>-8.6636098944881102E-4</v>
+      </c>
+      <c r="AS6" s="4">
+        <v>28.942275621855298</v>
+      </c>
+      <c r="AT6" s="4">
+        <v>3.8510460016514498</v>
+      </c>
+      <c r="AU6" s="4">
+        <v>-1.21026749044849</v>
+      </c>
+      <c r="AV6" s="4">
+        <v>35.509328934257098</v>
+      </c>
+      <c r="AW6" s="4">
+        <v>1.0900374375365001</v>
+      </c>
+      <c r="AX6" s="4">
+        <v>-3.7813379840972399</v>
+      </c>
+      <c r="AY6" s="4">
+        <v>19.675250680000001</v>
+      </c>
+      <c r="AZ6" s="4">
+        <v>-2.4947699499999998</v>
+      </c>
+      <c r="BA6" s="4">
+        <v>3.16268518</v>
+      </c>
+    </row>
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>12.157550364361301</v>
       </c>
@@ -1818,8 +3100,59 @@
       <c r="D7" s="4">
         <v>3.79386</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G7" s="4">
+        <v>25</v>
+      </c>
+      <c r="H7" s="4">
+        <v>25</v>
+      </c>
+      <c r="Y7" s="4">
+        <v>17.913580040012501</v>
+      </c>
+      <c r="Z7" s="4">
+        <v>14.306480065276901</v>
+      </c>
+      <c r="AA7" s="4">
+        <v>8.6726870460000001</v>
+      </c>
+      <c r="AP7" s="4">
+        <v>40.858774363473898</v>
+      </c>
+      <c r="AQ7" s="4">
+        <v>11.9793789019273</v>
+      </c>
+      <c r="AR7" s="4">
+        <v>14.9524769861109</v>
+      </c>
+      <c r="AS7" s="4">
+        <v>32.364452848225802</v>
+      </c>
+      <c r="AT7" s="4">
+        <v>12.3717423750247</v>
+      </c>
+      <c r="AU7" s="4">
+        <v>11.9686653894827</v>
+      </c>
+      <c r="AV7" s="4">
+        <v>37.792530135046803</v>
+      </c>
+      <c r="AW7" s="4">
+        <v>14.762299411040299</v>
+      </c>
+      <c r="AX7" s="4">
+        <v>13.0894550561184</v>
+      </c>
+      <c r="AY7" s="4">
+        <v>22.525664219999999</v>
+      </c>
+      <c r="AZ7" s="4">
+        <v>9.5536313909999997</v>
+      </c>
+      <c r="BA7" s="4">
+        <v>12.81628107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>14.760231648870301</v>
       </c>
@@ -1832,8 +3165,59 @@
       <c r="D8" s="4">
         <v>1.08396</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G8" s="4">
+        <v>30</v>
+      </c>
+      <c r="H8" s="4">
+        <v>30</v>
+      </c>
+      <c r="Y8" s="4">
+        <v>31.339461447313099</v>
+      </c>
+      <c r="Z8" s="4">
+        <v>25.017431907081399</v>
+      </c>
+      <c r="AA8" s="4">
+        <v>15.264089650000001</v>
+      </c>
+      <c r="AP8" s="4">
+        <v>42.513016739339498</v>
+      </c>
+      <c r="AQ8" s="4">
+        <v>52.8121040424111</v>
+      </c>
+      <c r="AR8" s="4">
+        <v>23.7861271793291</v>
+      </c>
+      <c r="AS8" s="4">
+        <v>35.496252180982701</v>
+      </c>
+      <c r="AT8" s="4">
+        <v>49.212037398324298</v>
+      </c>
+      <c r="AU8" s="4">
+        <v>25.349673977824601</v>
+      </c>
+      <c r="AV8" s="4">
+        <v>41.744535704265203</v>
+      </c>
+      <c r="AW8" s="4">
+        <v>54.886433931292501</v>
+      </c>
+      <c r="AX8" s="4">
+        <v>22.9798426548113</v>
+      </c>
+      <c r="AY8" s="4">
+        <v>23.412627430000001</v>
+      </c>
+      <c r="AZ8" s="4">
+        <v>37.441946739999999</v>
+      </c>
+      <c r="BA8" s="4">
+        <v>17.150709370000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>17.285082881441699</v>
       </c>
@@ -1846,8 +3230,59 @@
       <c r="D9" s="4">
         <v>7.2263999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G9" s="4">
+        <v>35</v>
+      </c>
+      <c r="H9" s="4">
+        <v>35</v>
+      </c>
+      <c r="Y9" s="4">
+        <v>31.354934388910799</v>
+      </c>
+      <c r="Z9" s="4">
+        <v>25.693460563374899</v>
+      </c>
+      <c r="AA9" s="4">
+        <v>16.93031878</v>
+      </c>
+      <c r="AP9" s="4">
+        <v>43.810561975230698</v>
+      </c>
+      <c r="AQ9" s="4">
+        <v>13.8249151130626</v>
+      </c>
+      <c r="AR9" s="4">
+        <v>-40.658303620800098</v>
+      </c>
+      <c r="AS9" s="4">
+        <v>34.916404346768402</v>
+      </c>
+      <c r="AT9" s="4">
+        <v>17.8680797404533</v>
+      </c>
+      <c r="AU9" s="4">
+        <v>-40.218053968421302</v>
+      </c>
+      <c r="AV9" s="4">
+        <v>41.834550714674997</v>
+      </c>
+      <c r="AW9" s="4">
+        <v>21.613285710188201</v>
+      </c>
+      <c r="AX9" s="4">
+        <v>-49.9137864189411</v>
+      </c>
+      <c r="AY9" s="4">
+        <v>24.06425406</v>
+      </c>
+      <c r="AZ9" s="4">
+        <v>12.314159869999999</v>
+      </c>
+      <c r="BA9" s="4">
+        <v>-26.710235600000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>19.7420591932039</v>
       </c>
@@ -1860,8 +3295,59 @@
       <c r="D10" s="4">
         <v>8.0392727374874298</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G10" s="4">
+        <v>40</v>
+      </c>
+      <c r="H10" s="4">
+        <v>40</v>
+      </c>
+      <c r="Y10" s="4">
+        <v>35.509328934257098</v>
+      </c>
+      <c r="Z10" s="4">
+        <v>28.942275621855298</v>
+      </c>
+      <c r="AA10" s="4">
+        <v>19.675250680000001</v>
+      </c>
+      <c r="AP10" s="4">
+        <v>46.403220698567999</v>
+      </c>
+      <c r="AQ10" s="4">
+        <v>-15.480847383522001</v>
+      </c>
+      <c r="AR10" s="4">
+        <v>21.314726589055901</v>
+      </c>
+      <c r="AS10" s="4">
+        <v>36.442330071055302</v>
+      </c>
+      <c r="AT10" s="4">
+        <v>-10.578810538261401</v>
+      </c>
+      <c r="AU10" s="4">
+        <v>18.051766147405999</v>
+      </c>
+      <c r="AV10" s="4">
+        <v>43.150765072798499</v>
+      </c>
+      <c r="AW10" s="4">
+        <v>-14.273735462744201</v>
+      </c>
+      <c r="AX10" s="4">
+        <v>19.4401398931141</v>
+      </c>
+      <c r="AY10" s="4">
+        <v>25.283719820000002</v>
+      </c>
+      <c r="AZ10" s="4">
+        <v>-7.0401488360000002</v>
+      </c>
+      <c r="BA10" s="4">
+        <v>19.343465890000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>22.139043572028001</v>
       </c>
@@ -1874,8 +3360,59 @@
       <c r="D11" s="4">
         <v>9.3203148870176609</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G11" s="4">
+        <v>45</v>
+      </c>
+      <c r="H11" s="4">
+        <v>45</v>
+      </c>
+      <c r="Y11" s="4">
+        <v>37.792530135046803</v>
+      </c>
+      <c r="Z11" s="4">
+        <v>32.364452848225802</v>
+      </c>
+      <c r="AA11" s="4">
+        <v>22.525664219999999</v>
+      </c>
+      <c r="AP11" s="4">
+        <v>52.826633416237897</v>
+      </c>
+      <c r="AQ11" s="4">
+        <v>43.512215505513403</v>
+      </c>
+      <c r="AR11" s="4">
+        <v>12.642323198841799</v>
+      </c>
+      <c r="AS11" s="4">
+        <v>44.2122094237901</v>
+      </c>
+      <c r="AT11" s="4">
+        <v>44.466171693571901</v>
+      </c>
+      <c r="AU11" s="4">
+        <v>11.062022408730099</v>
+      </c>
+      <c r="AV11" s="4">
+        <v>51.7579755991502</v>
+      </c>
+      <c r="AW11" s="4">
+        <v>47.968178256166297</v>
+      </c>
+      <c r="AX11" s="4">
+        <v>10.1233556644675</v>
+      </c>
+      <c r="AY11" s="4">
+        <v>31.316233050000001</v>
+      </c>
+      <c r="AZ11" s="4">
+        <v>33.489789950000002</v>
+      </c>
+      <c r="BA11" s="4">
+        <v>14.817256990000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>24.482416760248601</v>
       </c>
@@ -1888,8 +3425,59 @@
       <c r="D12" s="4">
         <v>12.8601264428573</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G12" s="4">
+        <v>50</v>
+      </c>
+      <c r="H12" s="4">
+        <v>50</v>
+      </c>
+      <c r="Y12" s="4">
+        <v>41.744535704265203</v>
+      </c>
+      <c r="Z12" s="4">
+        <v>35.496252180982701</v>
+      </c>
+      <c r="AA12" s="4">
+        <v>23.412627430000001</v>
+      </c>
+      <c r="AP12" s="4">
+        <v>52.930781940618502</v>
+      </c>
+      <c r="AQ12" s="4">
+        <v>48.347668850419701</v>
+      </c>
+      <c r="AR12" s="4">
+        <v>-16.0385558548296</v>
+      </c>
+      <c r="AS12" s="4">
+        <v>44.505769610168002</v>
+      </c>
+      <c r="AT12" s="4">
+        <v>46.057110496866599</v>
+      </c>
+      <c r="AU12" s="4">
+        <v>-14.412931164647899</v>
+      </c>
+      <c r="AV12" s="4">
+        <v>52.310025166339798</v>
+      </c>
+      <c r="AW12" s="4">
+        <v>53.114128191680997</v>
+      </c>
+      <c r="AX12" s="4">
+        <v>-21.829705200458299</v>
+      </c>
+      <c r="AY12" s="4">
+        <v>30.613827910000001</v>
+      </c>
+      <c r="AZ12" s="4">
+        <v>34.372535190000001</v>
+      </c>
+      <c r="BA12" s="4">
+        <v>-9.1771000489999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>26.7774381673444</v>
       </c>
@@ -1902,8 +3490,59 @@
       <c r="D13" s="4">
         <v>9.6408592305370906</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G13" s="4">
+        <v>55</v>
+      </c>
+      <c r="H13" s="4">
+        <v>55</v>
+      </c>
+      <c r="Y13" s="4">
+        <v>41.834550714674997</v>
+      </c>
+      <c r="Z13" s="4">
+        <v>34.916404346768402</v>
+      </c>
+      <c r="AA13" s="4">
+        <v>24.06425406</v>
+      </c>
+      <c r="AP13" s="4">
+        <v>53.705458975919498</v>
+      </c>
+      <c r="AQ13" s="4">
+        <v>-1.9567215069129</v>
+      </c>
+      <c r="AR13" s="4">
+        <v>-20.124040301285198</v>
+      </c>
+      <c r="AS13" s="4">
+        <v>43.653732903271099</v>
+      </c>
+      <c r="AT13" s="4">
+        <v>2.21410346158468</v>
+      </c>
+      <c r="AU13" s="4">
+        <v>-21.2084621450188</v>
+      </c>
+      <c r="AV13" s="4">
+        <v>51.557170758806201</v>
+      </c>
+      <c r="AW13" s="4">
+        <v>2.5048779664087499</v>
+      </c>
+      <c r="AX13" s="4">
+        <v>-27.650199397834498</v>
+      </c>
+      <c r="AY13" s="4">
+        <v>31.608791230000001</v>
+      </c>
+      <c r="AZ13" s="4">
+        <v>-1.966633318</v>
+      </c>
+      <c r="BA13" s="4">
+        <v>-10.388805400000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>29.028509630148999</v>
       </c>
@@ -1916,8 +3555,59 @@
       <c r="D14" s="4">
         <v>14.0589914796996</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G14" s="4">
+        <v>60</v>
+      </c>
+      <c r="H14" s="4">
+        <v>60</v>
+      </c>
+      <c r="Y14" s="4">
+        <v>43.150765072798499</v>
+      </c>
+      <c r="Z14" s="4">
+        <v>36.442330071055302</v>
+      </c>
+      <c r="AA14" s="4">
+        <v>25.283719820000002</v>
+      </c>
+      <c r="AP14" s="4">
+        <v>54.322688581342597</v>
+      </c>
+      <c r="AQ14" s="4">
+        <v>-0.18435148260936801</v>
+      </c>
+      <c r="AR14" s="4">
+        <v>0.52277297940945799</v>
+      </c>
+      <c r="AS14" s="4">
+        <v>43.973676156313601</v>
+      </c>
+      <c r="AT14" s="4">
+        <v>2.5831743087494399</v>
+      </c>
+      <c r="AU14" s="4">
+        <v>0.28711117230955102</v>
+      </c>
+      <c r="AV14" s="4">
+        <v>52.7445915281059</v>
+      </c>
+      <c r="AW14" s="4">
+        <v>2.1213624042501502</v>
+      </c>
+      <c r="AX14" s="4">
+        <v>-3.97862196082635</v>
+      </c>
+      <c r="AY14" s="4">
+        <v>30.725306570000001</v>
+      </c>
+      <c r="AZ14" s="4">
+        <v>-0.48456593799999997</v>
+      </c>
+      <c r="BA14" s="4">
+        <v>1.7498446459999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>31.239363532919398</v>
       </c>
@@ -1930,8 +3620,59 @@
       <c r="D15" s="4">
         <v>17.273257694797199</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G15" s="4">
+        <v>65</v>
+      </c>
+      <c r="H15" s="4">
+        <v>65</v>
+      </c>
+      <c r="Y15" s="4">
+        <v>51.7579755991502</v>
+      </c>
+      <c r="Z15" s="4">
+        <v>44.2122094237901</v>
+      </c>
+      <c r="AA15" s="4">
+        <v>31.316233050000001</v>
+      </c>
+      <c r="AP15" s="4">
+        <v>58.330714001573597</v>
+      </c>
+      <c r="AQ15" s="4">
+        <v>-40.502404175135801</v>
+      </c>
+      <c r="AR15" s="4">
+        <v>34.109432368691003</v>
+      </c>
+      <c r="AS15" s="4">
+        <v>47.456222555428603</v>
+      </c>
+      <c r="AT15" s="4">
+        <v>-38.232792483562697</v>
+      </c>
+      <c r="AU15" s="4">
+        <v>33.256893124850997</v>
+      </c>
+      <c r="AV15" s="4">
+        <v>56.319553627202303</v>
+      </c>
+      <c r="AW15" s="4">
+        <v>-41.527509323358402</v>
+      </c>
+      <c r="AX15" s="4">
+        <v>34.687276324065003</v>
+      </c>
+      <c r="AY15" s="4">
+        <v>32.943240250000002</v>
+      </c>
+      <c r="AZ15" s="4">
+        <v>-29.823332690000001</v>
+      </c>
+      <c r="BA15" s="4">
+        <v>24.67188414</v>
+      </c>
+    </row>
+    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>33.413200390998497</v>
       </c>
@@ -1944,8 +3685,59 @@
       <c r="D16" s="4">
         <v>17.036597781028799</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G16" s="4">
+        <v>70</v>
+      </c>
+      <c r="H16" s="4">
+        <v>70</v>
+      </c>
+      <c r="Y16" s="4">
+        <v>52.310025166339798</v>
+      </c>
+      <c r="Z16" s="4">
+        <v>44.505769610168002</v>
+      </c>
+      <c r="AA16" s="4">
+        <v>30.613827910000001</v>
+      </c>
+      <c r="AP16" s="4">
+        <v>58.594288513308797</v>
+      </c>
+      <c r="AQ16" s="4">
+        <v>10.519164130239</v>
+      </c>
+      <c r="AR16" s="4">
+        <v>-23.816766354586701</v>
+      </c>
+      <c r="AS16" s="4">
+        <v>48.780804319481902</v>
+      </c>
+      <c r="AT16" s="4">
+        <v>13.787067521823101</v>
+      </c>
+      <c r="AU16" s="4">
+        <v>-24.1840471830638</v>
+      </c>
+      <c r="AV16" s="4">
+        <v>57.065676205042799</v>
+      </c>
+      <c r="AW16" s="4">
+        <v>16.4636602605738</v>
+      </c>
+      <c r="AX16" s="4">
+        <v>-32.612381743300602</v>
+      </c>
+      <c r="AY16" s="4">
+        <v>34.482334369999997</v>
+      </c>
+      <c r="AZ16" s="4">
+        <v>8.2237457480000007</v>
+      </c>
+      <c r="BA16" s="4">
+        <v>-14.87055251</v>
+      </c>
+    </row>
+    <row r="17" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>35.552791671337303</v>
       </c>
@@ -1958,8 +3750,59 @@
       <c r="D17" s="4">
         <v>18.320840154538701</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G17" s="4">
+        <v>75</v>
+      </c>
+      <c r="H17" s="4">
+        <v>75</v>
+      </c>
+      <c r="Y17" s="4">
+        <v>51.557170758806201</v>
+      </c>
+      <c r="Z17" s="4">
+        <v>43.653732903271099</v>
+      </c>
+      <c r="AA17" s="4">
+        <v>31.608791230000001</v>
+      </c>
+      <c r="AP17" s="4">
+        <v>62.803105697604003</v>
+      </c>
+      <c r="AQ17" s="4">
+        <v>28.507392666181001</v>
+      </c>
+      <c r="AR17" s="4">
+        <v>57.728458422472499</v>
+      </c>
+      <c r="AS17" s="4">
+        <v>53.236499913979998</v>
+      </c>
+      <c r="AT17" s="4">
+        <v>32.769018536581399</v>
+      </c>
+      <c r="AU17" s="4">
+        <v>53.924747397921401</v>
+      </c>
+      <c r="AV17" s="4">
+        <v>61.771962973055899</v>
+      </c>
+      <c r="AW17" s="4">
+        <v>34.0692850206188</v>
+      </c>
+      <c r="AX17" s="4">
+        <v>59.422690474543998</v>
+      </c>
+      <c r="AY17" s="4">
+        <v>37.487123910000001</v>
+      </c>
+      <c r="AZ17" s="4">
+        <v>26.477786779999999</v>
+      </c>
+      <c r="BA17" s="4">
+        <v>45.117494020000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>37.660558090522102</v>
       </c>
@@ -1972,8 +3815,59 @@
       <c r="D18" s="4">
         <v>20.203385416422901</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G18" s="4">
+        <v>80</v>
+      </c>
+      <c r="H18" s="4">
+        <v>80</v>
+      </c>
+      <c r="Y18" s="4">
+        <v>52.7445915281059</v>
+      </c>
+      <c r="Z18" s="4">
+        <v>43.973676156313601</v>
+      </c>
+      <c r="AA18" s="4">
+        <v>30.725306570000001</v>
+      </c>
+      <c r="AP18" s="4">
+        <v>68.3412110813655</v>
+      </c>
+      <c r="AQ18" s="4">
+        <v>12.532870267761</v>
+      </c>
+      <c r="AR18" s="4">
+        <v>16.419202413412499</v>
+      </c>
+      <c r="AS18" s="4">
+        <v>57.781999474018399</v>
+      </c>
+      <c r="AT18" s="4">
+        <v>16.212526570737399</v>
+      </c>
+      <c r="AU18" s="4">
+        <v>14.7866637730371</v>
+      </c>
+      <c r="AV18" s="4">
+        <v>67.121690575514293</v>
+      </c>
+      <c r="AW18" s="4">
+        <v>16.451667850886999</v>
+      </c>
+      <c r="AX18" s="4">
+        <v>13.329449401459501</v>
+      </c>
+      <c r="AY18" s="4">
+        <v>41.748003009999998</v>
+      </c>
+      <c r="AZ18" s="4">
+        <v>10.20374185</v>
+      </c>
+      <c r="BA18" s="4">
+        <v>16.00373604</v>
+      </c>
+    </row>
+    <row r="19" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>39.738630230206802</v>
       </c>
@@ -1986,8 +3880,59 @@
       <c r="D19" s="4">
         <v>20.634885666407001</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G19" s="4">
+        <v>85</v>
+      </c>
+      <c r="H19" s="4">
+        <v>85</v>
+      </c>
+      <c r="Y19" s="4">
+        <v>56.319553627202303</v>
+      </c>
+      <c r="Z19" s="4">
+        <v>47.456222555428603</v>
+      </c>
+      <c r="AA19" s="4">
+        <v>32.943240250000002</v>
+      </c>
+      <c r="AP19" s="4">
+        <v>68.635025805353095</v>
+      </c>
+      <c r="AQ19" s="4">
+        <v>8.9439994577222796E-3</v>
+      </c>
+      <c r="AR19" s="4">
+        <v>-1.33533717872059E-3</v>
+      </c>
+      <c r="AS19" s="4">
+        <v>57.790494199513198</v>
+      </c>
+      <c r="AT19" s="4">
+        <v>2.6980410335832898</v>
+      </c>
+      <c r="AU19" s="4">
+        <v>-0.25632901353320697</v>
+      </c>
+      <c r="AV19" s="4">
+        <v>67.798100176184406</v>
+      </c>
+      <c r="AW19" s="4">
+        <v>3.0429957310567599</v>
+      </c>
+      <c r="AX19" s="4">
+        <v>-5.7688032873011199</v>
+      </c>
+      <c r="AY19" s="4">
+        <v>41.18961891</v>
+      </c>
+      <c r="AZ19" s="4">
+        <v>-0.20911776400000001</v>
+      </c>
+      <c r="BA19" s="4">
+        <v>2.0307955629999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>41.7888961531891</v>
       </c>
@@ -2000,8 +3945,59 @@
       <c r="D20" s="4">
         <v>21.244943559407499</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G20" s="4">
+        <v>90</v>
+      </c>
+      <c r="H20" s="4">
+        <v>90</v>
+      </c>
+      <c r="Y20" s="4">
+        <v>57.065676205042799</v>
+      </c>
+      <c r="Z20" s="4">
+        <v>48.780804319481902</v>
+      </c>
+      <c r="AA20" s="4">
+        <v>34.482334369999997</v>
+      </c>
+      <c r="AP20" s="4">
+        <v>73.091809568476606</v>
+      </c>
+      <c r="AQ20" s="4">
+        <v>-30.400964455216201</v>
+      </c>
+      <c r="AR20" s="4">
+        <v>0.87663903384140895</v>
+      </c>
+      <c r="AS20" s="4">
+        <v>62.229008458145699</v>
+      </c>
+      <c r="AT20" s="4">
+        <v>-26.473980444513899</v>
+      </c>
+      <c r="AU20" s="4">
+        <v>6.4705959731692395E-2</v>
+      </c>
+      <c r="AV20" s="4">
+        <v>72.206954570721905</v>
+      </c>
+      <c r="AW20" s="4">
+        <v>-28.146097517718498</v>
+      </c>
+      <c r="AX20" s="4">
+        <v>-5.3524793115277802</v>
+      </c>
+      <c r="AY20" s="4">
+        <v>44.802764119999999</v>
+      </c>
+      <c r="AZ20" s="4">
+        <v>-20.67342206</v>
+      </c>
+      <c r="BA20" s="4">
+        <v>3.7981022719999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43.813039297706297</v>
       </c>
@@ -2014,8 +4010,59 @@
       <c r="D21" s="4">
         <v>23.8360556408559</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G21" s="4">
+        <v>95</v>
+      </c>
+      <c r="H21" s="4">
+        <v>95</v>
+      </c>
+      <c r="Y21" s="4">
+        <v>61.771962973055899</v>
+      </c>
+      <c r="Z21" s="4">
+        <v>53.236499913979998</v>
+      </c>
+      <c r="AA21" s="4">
+        <v>37.487123910000001</v>
+      </c>
+      <c r="AP21" s="4">
+        <v>73.460038120237598</v>
+      </c>
+      <c r="AQ21" s="4">
+        <v>12.832503955958799</v>
+      </c>
+      <c r="AR21" s="4">
+        <v>66.1053807048321</v>
+      </c>
+      <c r="AS21" s="4">
+        <v>62.790814232688398</v>
+      </c>
+      <c r="AT21" s="4">
+        <v>17.1984927210693</v>
+      </c>
+      <c r="AU21" s="4">
+        <v>64.8789164532417</v>
+      </c>
+      <c r="AV21" s="4">
+        <v>72.670393280597295</v>
+      </c>
+      <c r="AW21" s="4">
+        <v>17.670801846078302</v>
+      </c>
+      <c r="AX21" s="4">
+        <v>68.999838748284105</v>
+      </c>
+      <c r="AY21" s="4">
+        <v>45.417334719999999</v>
+      </c>
+      <c r="AZ21" s="4">
+        <v>14.050158270000001</v>
+      </c>
+      <c r="BA21" s="4">
+        <v>52.820308879999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>45.812568988870296</v>
       </c>
@@ -2028,8 +4075,59 @@
       <c r="D22" s="4">
         <v>25.713404819257299</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G22" s="4">
+        <v>100</v>
+      </c>
+      <c r="H22" s="4">
+        <v>100</v>
+      </c>
+      <c r="Y22" s="4">
+        <v>67.121690575514293</v>
+      </c>
+      <c r="Z22" s="4">
+        <v>57.781999474018399</v>
+      </c>
+      <c r="AA22" s="4">
+        <v>41.748003009999998</v>
+      </c>
+      <c r="AP22" s="4">
+        <v>73.973784381781797</v>
+      </c>
+      <c r="AQ22" s="4">
+        <v>-26.325365684185901</v>
+      </c>
+      <c r="AR22" s="4">
+        <v>57.542881474278303</v>
+      </c>
+      <c r="AS22" s="4">
+        <v>62.520762952460402</v>
+      </c>
+      <c r="AT22" s="4">
+        <v>-22.9027796990304</v>
+      </c>
+      <c r="AU22" s="4">
+        <v>57.676003415602302</v>
+      </c>
+      <c r="AV22" s="4">
+        <v>72.613740508446696</v>
+      </c>
+      <c r="AW22" s="4">
+        <v>-25.7818124235407</v>
+      </c>
+      <c r="AX22" s="4">
+        <v>60.847140135161801</v>
+      </c>
+      <c r="AY22" s="4">
+        <v>44.977400539999998</v>
+      </c>
+      <c r="AZ22" s="4">
+        <v>-15.759297760000001</v>
+      </c>
+      <c r="BA22" s="4">
+        <v>46.867128729999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>47.788845265682497</v>
       </c>
@@ -2042,8 +4140,53 @@
       <c r="D23" s="4">
         <v>26.8484222103897</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="Y23" s="4">
+        <v>67.798100176184406</v>
+      </c>
+      <c r="Z23" s="4">
+        <v>57.790494199513198</v>
+      </c>
+      <c r="AA23" s="4">
+        <v>41.18961891</v>
+      </c>
+      <c r="AP23" s="4">
+        <v>82.424217104485194</v>
+      </c>
+      <c r="AQ23" s="4">
+        <v>1.0401203710153101E-2</v>
+      </c>
+      <c r="AR23" s="4">
+        <v>-1.55289745749077E-3</v>
+      </c>
+      <c r="AS23" s="4">
+        <v>71.363000178237201</v>
+      </c>
+      <c r="AT23" s="4">
+        <v>2.4231453688000602</v>
+      </c>
+      <c r="AU23" s="4">
+        <v>-0.144987042294309</v>
+      </c>
+      <c r="AV23" s="4">
+        <v>82.852522013889995</v>
+      </c>
+      <c r="AW23" s="4">
+        <v>3.93871381203753</v>
+      </c>
+      <c r="AX23" s="4">
+        <v>-6.8866732419259096</v>
+      </c>
+      <c r="AY23" s="4">
+        <v>51.5533705</v>
+      </c>
+      <c r="AZ23" s="4">
+        <v>-0.22631556899999999</v>
+      </c>
+      <c r="BA23" s="4">
+        <v>2.455484518</v>
+      </c>
+    </row>
+    <row r="24" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>49.743099276495997</v>
       </c>
@@ -2056,8 +4199,53 @@
       <c r="D24" s="4">
         <v>27.709507851675699</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="Y24" s="4">
+        <v>72.206954570721905</v>
+      </c>
+      <c r="Z24" s="4">
+        <v>62.229008458145699</v>
+      </c>
+      <c r="AA24" s="4">
+        <v>44.802764119999999</v>
+      </c>
+      <c r="AP24" s="4">
+        <v>82.7944957735874</v>
+      </c>
+      <c r="AQ24" s="4">
+        <v>-2.6193590588732798</v>
+      </c>
+      <c r="AR24" s="4">
+        <v>78.916378509536599</v>
+      </c>
+      <c r="AS24" s="4">
+        <v>71.728079207486402</v>
+      </c>
+      <c r="AT24" s="4">
+        <v>2.00251255881073</v>
+      </c>
+      <c r="AU24" s="4">
+        <v>79.476013871425195</v>
+      </c>
+      <c r="AV24" s="4">
+        <v>82.710924759429204</v>
+      </c>
+      <c r="AW24" s="4">
+        <v>9.3396308130988495E-2</v>
+      </c>
+      <c r="AX24" s="4">
+        <v>85.818920002410394</v>
+      </c>
+      <c r="AY24" s="4">
+        <v>51.578697480000002</v>
+      </c>
+      <c r="AZ24" s="4">
+        <v>0.74805048100000004</v>
+      </c>
+      <c r="BA24" s="4">
+        <v>60.979802960000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>51.676450180349299</v>
       </c>
@@ -2070,8 +4258,53 @@
       <c r="D25" s="4">
         <v>29.4376797813505</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="Y25" s="4">
+        <v>72.670393280597295</v>
+      </c>
+      <c r="Z25" s="4">
+        <v>62.790814232688398</v>
+      </c>
+      <c r="AA25" s="4">
+        <v>45.417334719999999</v>
+      </c>
+      <c r="AP25" s="4">
+        <v>95.816325481331205</v>
+      </c>
+      <c r="AQ25" s="4">
+        <v>-0.48581333227337697</v>
+      </c>
+      <c r="AR25" s="4">
+        <v>2.3214451067672401</v>
+      </c>
+      <c r="AS25" s="4">
+        <v>84.665480396724107</v>
+      </c>
+      <c r="AT25" s="4">
+        <v>2.0277158371464501</v>
+      </c>
+      <c r="AU25" s="4">
+        <v>2.1902626313462998</v>
+      </c>
+      <c r="AV25" s="4">
+        <v>97.4521674453065</v>
+      </c>
+      <c r="AW25" s="4">
+        <v>3.9348360015589199</v>
+      </c>
+      <c r="AX25" s="4">
+        <v>-4.3928147494715297</v>
+      </c>
+      <c r="AY25" s="4">
+        <v>61.769095489999998</v>
+      </c>
+      <c r="AZ25" s="4">
+        <v>-0.868615052</v>
+      </c>
+      <c r="BA25" s="4">
+        <v>4.3396509989999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>53.589919264710403</v>
       </c>
@@ -2084,8 +4317,17 @@
       <c r="D26" s="4">
         <v>31.3239783844108</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="Y26" s="4">
+        <v>72.613740508446696</v>
+      </c>
+      <c r="Z26" s="4">
+        <v>62.520762952460402</v>
+      </c>
+      <c r="AA26" s="4">
+        <v>44.977400539999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>55.4844418246023</v>
       </c>
@@ -2098,8 +4340,17 @@
       <c r="D27" s="4">
         <v>31.829663840795099</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="Y27" s="4">
+        <v>82.852522013889995</v>
+      </c>
+      <c r="Z27" s="4">
+        <v>71.363000178237201</v>
+      </c>
+      <c r="AA27" s="4">
+        <v>51.5533705</v>
+      </c>
+    </row>
+    <row r="28" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>57.360877225658697</v>
       </c>
@@ -2112,8 +4363,17 @@
       <c r="D28" s="4">
         <v>33.135553577356802</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="Y28" s="4">
+        <v>82.710924759429204</v>
+      </c>
+      <c r="Z28" s="4">
+        <v>71.728079207486402</v>
+      </c>
+      <c r="AA28" s="4">
+        <v>51.578697480000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>59.220017482019998</v>
       </c>
@@ -2126,8 +4386,17 @@
       <c r="D29" s="4">
         <v>35.103035066479997</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="Y29" s="4">
+        <v>97.4521674453065</v>
+      </c>
+      <c r="Z29" s="4">
+        <v>84.665480396724107</v>
+      </c>
+      <c r="AA29" s="4">
+        <v>61.769095489999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>61.062594610629297</v>
       </c>
@@ -2141,7 +4410,7 @@
         <v>36.022773456836397</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>62.889286970436302</v>
       </c>
@@ -2155,7 +4424,7 @@
         <v>38.021310290524497</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>64.700724754063202</v>
       </c>
@@ -2395,16 +4664,16 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>93.611191018306599</v>
+        <v>96.822045162958503</v>
       </c>
       <c r="B49" s="2">
-        <v>90.211035887826696</v>
+        <v>93.878806202783693</v>
       </c>
       <c r="C49" s="3">
-        <v>78.122318625670104</v>
+        <v>81.071228937973899</v>
       </c>
       <c r="D49" s="4">
-        <v>60.816914677161797</v>
+        <v>63.565411097727697</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -2423,30 +4692,30 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>96.822045162958503</v>
+        <v>98.415036972298196</v>
       </c>
       <c r="B51" s="2">
-        <v>93.878806202783693</v>
+        <v>95.526065888121096</v>
       </c>
       <c r="C51" s="3">
-        <v>81.071228937973899</v>
+        <v>82.636111340414203</v>
       </c>
       <c r="D51" s="4">
-        <v>63.565411097727697</v>
+        <v>64.403088913774198</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>98.415036972298196</v>
+        <v>93.611191018306599</v>
       </c>
       <c r="B52" s="2">
-        <v>95.526065888121096</v>
+        <v>90.211035887826696</v>
       </c>
       <c r="C52" s="3">
-        <v>82.636111340414203</v>
+        <v>78.122318625670104</v>
       </c>
       <c r="D52" s="4">
-        <v>64.403088913774198</v>
+        <v>60.816914677161797</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -2473,7 +4742,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>